<commit_message>
update socket and zns
</commit_message>
<xml_diff>
--- a/public/assets/files/sample_export.xlsx
+++ b/public/assets/files/sample_export.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PHANMEM_THO\alotaxi-project\main\alotaxi-v2\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E692440-D5C5-4053-A491-1AC5D5D6D956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8672B66-1227-40E0-858E-39F86F03912A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="814" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -606,7 +606,7 @@
     <col min="2" max="2" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="2" customWidth="1"/>
     <col min="6" max="6" width="72.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="31.85546875" style="1"/>
   </cols>

</xml_diff>

<commit_message>
update change password and add discount
</commit_message>
<xml_diff>
--- a/public/assets/files/sample_export.xlsx
+++ b/public/assets/files/sample_export.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PHANMEM_THO\alotaxi-project\main\alotaxi-v2\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8672B66-1227-40E0-858E-39F86F03912A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6695B755-C7FA-4EE1-9F9D-2464B21D27C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="814" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -134,7 +134,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -170,43 +170,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -224,7 +187,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -246,9 +209,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -267,14 +227,14 @@
     <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -597,12 +557,12 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -631,33 +591,30 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+    <row r="2" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17">
         <v>1</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="14"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="16" t="s">
+      <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="11">
-        <f>SUM(E2:E2)</f>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="10">
+        <f ca="1">SUM(E2:INDIRECT("E"&amp;ROW()-1))</f>
         <v>0</v>
       </c>
-      <c r="F3" s="12"/>
+      <c r="F3" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:D3"/>
-  </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="88" firstPageNumber="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>